<commit_message>
2D arrays and dataframes
</commit_message>
<xml_diff>
--- a/FY24 Projects DRAFT-v2.xlsx
+++ b/FY24 Projects DRAFT-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsteel01\Box\01 - P Drive 2\Employment\Goals\FY24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AF2CC7-2E35-418F-8587-0AF38E96DDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D174454-A822-4DBE-84CE-8FBF9CBAB2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A9DDD929-39F7-4D1E-ADFC-1FBC098A0B9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>task</t>
   </si>
@@ -80,12 +80,6 @@
     <t xml:space="preserve">loan rule Code4Lib article and collaboration with Getty </t>
   </si>
   <si>
-    <t>open access work from Chris?</t>
-  </si>
-  <si>
-    <t>Alma Primo COP Fulfillment Zone</t>
-  </si>
-  <si>
     <t>EAD exporter app re-enable</t>
   </si>
   <si>
@@ -128,58 +122,61 @@
     <t>2024-05-31</t>
   </si>
   <si>
-    <t>2023-12-31</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
     <t>2024-01-01</t>
   </si>
   <si>
-    <t>2024-01-31</t>
-  </si>
-  <si>
     <t>2023-11-01</t>
   </si>
   <si>
-    <t>2024-09-01</t>
-  </si>
-  <si>
-    <t>2025-04-01</t>
-  </si>
-  <si>
     <t>ASPace serve static EADs</t>
   </si>
   <si>
-    <t>2024-02-01</t>
-  </si>
-  <si>
-    <t>2024-06-01</t>
-  </si>
-  <si>
     <t>2024-08-01</t>
   </si>
   <si>
     <t>2024-04-30</t>
   </si>
   <si>
-    <t>2024-03-01</t>
-  </si>
-  <si>
     <t>2024-02-28</t>
   </si>
   <si>
-    <t>2024-03-31</t>
-  </si>
-  <si>
     <t>2024-07-01</t>
   </si>
   <si>
-    <t>2024-07-31</t>
-  </si>
-  <si>
     <t>level_of_effort</t>
+  </si>
+  <si>
+    <t>2023-10-08</t>
+  </si>
+  <si>
+    <t>2023-11-15</t>
+  </si>
+  <si>
+    <t>2023-12-01</t>
+  </si>
+  <si>
+    <t>2023-12-30</t>
+  </si>
+  <si>
+    <t>2024-01-15</t>
+  </si>
+  <si>
+    <t>2024-01-30</t>
+  </si>
+  <si>
+    <t>2024-08-02</t>
+  </si>
+  <si>
+    <t>2024-08-30</t>
+  </si>
+  <si>
+    <t>2024-07-30</t>
+  </si>
+  <si>
+    <t>2024-04-10</t>
+  </si>
+  <si>
+    <t>2024-06-10</t>
   </si>
 </sst>
 </file>
@@ -546,11 +543,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2CE495-DA38-4754-9DAE-496F22D67360}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -579,10 +576,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -593,10 +590,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -607,10 +604,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -621,10 +618,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -632,13 +629,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -646,16 +643,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -663,13 +660,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -677,10 +674,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -691,13 +688,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -705,10 +702,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -719,13 +716,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -733,10 +730,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -747,24 +744,24 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -772,64 +769,36 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C19">
-    <sortCondition ref="B2:B19"/>
-    <sortCondition ref="C2:C19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
+    <sortCondition ref="B2:B17"/>
+    <sortCondition ref="C2:C17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>